<commit_message>
atlas 2.2 cmd ref
</commit_message>
<xml_diff>
--- a/doc/api_mapping.xlsx
+++ b/doc/api_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10419"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10424"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taygan/Documents/Developer/purviewcli/purviewcli/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99F0CC1-2F9E-0444-9BD7-DA862E589A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550C5DE1-D943-E141-92E0-A3CBC5A58055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping" sheetId="1" r:id="rId1"/>
@@ -3102,9 +3102,6 @@
     <t>pv entity addLabels --guid=&lt;val&gt; --payloadFile=&lt;val&gt;</t>
   </si>
   <si>
-    <t>pv entity deleteLabels --guid=&lt;val&gt;</t>
-  </si>
-  <si>
     <t>pv entity setLabels --guid=&lt;val&gt; --payloadFile=&lt;val&gt;</t>
   </si>
   <si>
@@ -3115,6 +3112,9 @@
   </si>
   <si>
     <t>pv entity setLabelsByUniqueAttribute --typeName=&lt;val&gt; --qualifiedName=&lt;val&gt; --payloadFile=&lt;val&gt;</t>
+  </si>
+  <si>
+    <t>pv entity deleteLabels --guid=&lt;val&gt; --payloadFile=&lt;val&gt;</t>
   </si>
 </sst>
 </file>
@@ -3751,7 +3751,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3787,16 +3787,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3843,127 +3838,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -4225,6 +4100,46 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4239,23 +4154,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F11FDB1-5E01-487A-9C37-FAA9F7174453}" name="Table1" displayName="Table1" ref="A1:K199" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
-  <autoFilter ref="A1:K199" xr:uid="{7F11FDB1-5E01-487A-9C37-FAA9F7174453}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F11FDB1-5E01-487A-9C37-FAA9F7174453}" name="Table1" displayName="Table1" ref="A1:K199" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K199">
     <sortCondition ref="H1:H199"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{87EB5FFA-5DF0-4B94-BF81-FC009D6463B2}" name="ID" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{7924792E-FE42-4479-B48B-F5BE66B74CB2}" name="H1" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{58F5661A-03C7-4BC2-8B19-2C0C541A692C}" name="H2" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{982580AD-224D-43FC-9E13-2D4C03B80920}" name="H3" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{8846B3E0-E6D0-4069-97FD-9F2A2295AB08}" name="DESCRIPTION" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{B182668B-622A-477A-8A1A-5BBFD75F305A}" name="DOCUMENTATION" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{59A849C9-9B58-4DDD-8588-D6463C2864C7}" name="METHOD" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{0F299357-521B-43E5-9B71-A55AA4CDF468}" name="ENDPOINT" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{4ACDF120-F277-4CCA-A233-63A53A220CF5}" name="API_VERSION" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{DFCF8009-8B07-4BAC-B0DC-08B99BADF19D}" name="PARAMS" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{06B6125B-6314-49C0-AC81-EA26DAEE9302}" name="PURVIEWCLI" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{87EB5FFA-5DF0-4B94-BF81-FC009D6463B2}" name="ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{7924792E-FE42-4479-B48B-F5BE66B74CB2}" name="H1" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{58F5661A-03C7-4BC2-8B19-2C0C541A692C}" name="H2" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{982580AD-224D-43FC-9E13-2D4C03B80920}" name="H3" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{8846B3E0-E6D0-4069-97FD-9F2A2295AB08}" name="DESCRIPTION" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{B182668B-622A-477A-8A1A-5BBFD75F305A}" name="DOCUMENTATION" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{59A849C9-9B58-4DDD-8588-D6463C2864C7}" name="METHOD" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{0F299357-521B-43E5-9B71-A55AA4CDF468}" name="ENDPOINT" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4ACDF120-F277-4CCA-A233-63A53A220CF5}" name="API_VERSION" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{DFCF8009-8B07-4BAC-B0DC-08B99BADF19D}" name="PARAMS" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{06B6125B-6314-49C0-AC81-EA26DAEE9302}" name="PURVIEWCLI" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4571,8 +4485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K199"/>
   <sheetViews>
-    <sheetView topLeftCell="B26" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5344,10 +5258,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -5359,7 +5273,7 @@
       <c r="F23" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H23" s="5" t="s">
@@ -5375,10 +5289,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -5390,7 +5304,7 @@
       <c r="F24" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H24" s="5" t="s">
@@ -5510,10 +5424,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -5525,7 +5439,7 @@
       <c r="F28" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H28" s="5" t="s">
@@ -5543,10 +5457,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -5558,7 +5472,7 @@
       <c r="F29" s="5" t="s">
         <v>980</v>
       </c>
-      <c r="G29" s="23" t="s">
+      <c r="G29" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H29" s="5" t="s">
@@ -5574,10 +5488,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D30" s="6" t="s">
@@ -5589,7 +5503,7 @@
       <c r="F30" s="5" t="s">
         <v>982</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H30" s="5" t="s">
@@ -5605,10 +5519,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -5620,7 +5534,7 @@
       <c r="F31" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="G31" s="23" t="s">
+      <c r="G31" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="5" t="s">
@@ -5840,10 +5754,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D38" s="6" t="s">
@@ -5855,7 +5769,7 @@
       <c r="F38" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="G38" s="23" t="s">
+      <c r="G38" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H38" s="5" t="s">
@@ -5871,10 +5785,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -5886,7 +5800,7 @@
       <c r="F39" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="G39" s="23" t="s">
+      <c r="G39" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H39" s="5" t="s">
@@ -5902,10 +5816,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -5917,7 +5831,7 @@
       <c r="F40" s="5" t="s">
         <v>977</v>
       </c>
-      <c r="G40" s="23" t="s">
+      <c r="G40" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H40" s="5" t="s">
@@ -6137,10 +6051,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="8"/>
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -6152,7 +6066,7 @@
       <c r="F47" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="G47" s="23" t="s">
+      <c r="G47" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H47" s="5" t="s">
@@ -6170,10 +6084,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D48" s="6" t="s">
@@ -6185,7 +6099,7 @@
       <c r="F48" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="G48" s="23" t="s">
+      <c r="G48" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H48" s="5" t="s">
@@ -6203,10 +6117,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="8"/>
-      <c r="B49" s="27" t="s">
+      <c r="B49" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="C49" s="27" t="s">
         <v>489</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -6218,7 +6132,7 @@
       <c r="F49" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="G49" s="23" t="s">
+      <c r="G49" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H49" s="5" t="s">
@@ -10360,7 +10274,7 @@
       <c r="H178" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="I178" s="25" t="s">
+      <c r="I178" s="24" t="s">
         <v>278</v>
       </c>
       <c r="J178" s="3"/>
@@ -10394,7 +10308,7 @@
       <c r="H179" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="I179" s="24" t="s">
+      <c r="I179" s="23" t="s">
         <v>278</v>
       </c>
       <c r="J179" s="2"/>
@@ -10428,7 +10342,7 @@
       <c r="H180" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="I180" s="24" t="s">
+      <c r="I180" s="23" t="s">
         <v>278</v>
       </c>
       <c r="J180" s="2"/>
@@ -10460,7 +10374,7 @@
       <c r="H181" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I181" s="24" t="s">
+      <c r="I181" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J181" s="2" t="s">
@@ -10494,7 +10408,7 @@
       <c r="H182" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I182" s="24" t="s">
+      <c r="I182" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J182" s="2"/>
@@ -10526,7 +10440,7 @@
       <c r="H183" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="I183" s="24" t="s">
+      <c r="I183" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J183" s="2" t="s">
@@ -10560,7 +10474,7 @@
       <c r="H184" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I184" s="24" t="s">
+      <c r="I184" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J184" s="2"/>
@@ -10592,7 +10506,7 @@
       <c r="H185" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I185" s="26" t="s">
+      <c r="I185" s="25" t="s">
         <v>609</v>
       </c>
       <c r="J185" s="4"/>
@@ -10624,7 +10538,7 @@
       <c r="H186" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I186" s="24" t="s">
+      <c r="I186" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J186" s="2"/>
@@ -10656,7 +10570,7 @@
       <c r="H187" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I187" s="24" t="s">
+      <c r="I187" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J187" s="2"/>
@@ -10688,7 +10602,7 @@
       <c r="H188" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I188" s="24" t="s">
+      <c r="I188" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J188" s="2"/>
@@ -10720,7 +10634,7 @@
       <c r="H189" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I189" s="24" t="s">
+      <c r="I189" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J189" s="2"/>
@@ -10752,7 +10666,7 @@
       <c r="H190" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I190" s="24" t="s">
+      <c r="I190" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J190" s="2"/>
@@ -10784,7 +10698,7 @@
       <c r="H191" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I191" s="24" t="s">
+      <c r="I191" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J191" s="2"/>
@@ -10816,7 +10730,7 @@
       <c r="H192" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I192" s="24" t="s">
+      <c r="I192" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J192" s="2"/>
@@ -10845,10 +10759,10 @@
       <c r="G193" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H193" s="30" t="s">
+      <c r="H193" t="s">
         <v>54</v>
       </c>
-      <c r="I193" s="24" t="s">
+      <c r="I193" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J193" s="2"/>
@@ -10880,7 +10794,7 @@
       <c r="H194" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="I194" s="24" t="s">
+      <c r="I194" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J194" s="2"/>
@@ -10909,10 +10823,10 @@
       <c r="G195" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H195" s="29" t="s">
+      <c r="H195" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="I195" s="24" t="s">
+      <c r="I195" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J195" s="2"/>
@@ -10944,7 +10858,7 @@
       <c r="H196" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="I196" s="24" t="s">
+      <c r="I196" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J196" s="2"/>
@@ -10976,7 +10890,7 @@
       <c r="H197" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="I197" s="24" t="s">
+      <c r="I197" s="23" t="s">
         <v>609</v>
       </c>
       <c r="J197" s="2"/>
@@ -11008,7 +10922,7 @@
       <c r="H198" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="I198" s="26" t="s">
+      <c r="I198" s="25" t="s">
         <v>609</v>
       </c>
       <c r="J198" s="4"/>
@@ -11040,7 +10954,7 @@
       <c r="H199" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="I199" s="26" t="s">
+      <c r="I199" s="25" t="s">
         <v>609</v>
       </c>
       <c r="J199" s="4"/>
@@ -11051,16 +10965,16 @@
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="G2:G199">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"GET"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"PUT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"POST"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"DELETE"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11080,8 +10994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D3487-705C-4F00-B617-2E126542661E}">
   <dimension ref="A1:B180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170"/>
+    <sheetView topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12495,7 +12409,7 @@
         <v>995</v>
       </c>
       <c r="B176" t="s">
-        <v>1021</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
@@ -12503,7 +12417,7 @@
         <v>996</v>
       </c>
       <c r="B177" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
@@ -12511,7 +12425,7 @@
         <v>997</v>
       </c>
       <c r="B178" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
@@ -12519,7 +12433,7 @@
         <v>998</v>
       </c>
       <c r="B179" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
@@ -12527,7 +12441,7 @@
         <v>999</v>
       </c>
       <c r="B180" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>